<commit_message>
updated with Lyra and Ludmera
</commit_message>
<xml_diff>
--- a/src/assets/echocalypse_cases.xlsx
+++ b/src/assets/echocalypse_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\echocalypse-front\TheRealPlagiariser\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8228336-B2C4-4B0E-94E6-04EE109067F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D354FE81-7D14-4C7D-B21F-C8CCE630B73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5505" yWindow="3405" windowWidth="28800" windowHeight="15435" xr2:uid="{1E519EE2-4CBB-4C35-ACD1-DF17E43DC2A8}"/>
+    <workbookView xWindow="5340" yWindow="3855" windowWidth="28800" windowHeight="15435" xr2:uid="{1E519EE2-4CBB-4C35-ACD1-DF17E43DC2A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="137">
   <si>
     <t>IsInGlobal</t>
   </si>
@@ -433,6 +433,18 @@
   </si>
   <si>
     <t>Raeon,Chiraha</t>
+  </si>
+  <si>
+    <t>Lyra</t>
+  </si>
+  <si>
+    <t>Ludmera</t>
+  </si>
+  <si>
+    <t>Mori,Aiken</t>
+  </si>
+  <si>
+    <t>Mordred,Camelia</t>
   </si>
 </sst>
 </file>
@@ -814,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05404559-8E4A-4D78-AA1A-747D26FBBE70}">
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="J62" sqref="J62"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="L55" sqref="L55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2820,71 +2832,71 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="B63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C63" t="s">
-        <v>127</v>
-      </c>
-      <c r="D63" t="s">
-        <v>127</v>
+        <v>27</v>
+      </c>
+      <c r="D63">
+        <v>11</v>
       </c>
       <c r="E63" t="s">
-        <v>127</v>
-      </c>
-      <c r="F63" t="s">
-        <v>127</v>
+        <v>131</v>
+      </c>
+      <c r="F63">
+        <v>5</v>
       </c>
       <c r="G63" t="s">
-        <v>127</v>
-      </c>
-      <c r="H63" t="s">
-        <v>127</v>
+        <v>136</v>
+      </c>
+      <c r="H63">
+        <v>11</v>
       </c>
       <c r="I63" t="s">
-        <v>127</v>
-      </c>
-      <c r="J63" t="s">
-        <v>127</v>
+        <v>56</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C64" t="s">
-        <v>127</v>
-      </c>
-      <c r="D64" t="s">
-        <v>127</v>
+        <v>133</v>
+      </c>
+      <c r="D64">
+        <v>5</v>
       </c>
       <c r="E64" t="s">
-        <v>127</v>
-      </c>
-      <c r="F64" t="s">
-        <v>127</v>
+        <v>60</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
       </c>
       <c r="G64" t="s">
-        <v>127</v>
-      </c>
-      <c r="H64" t="s">
-        <v>127</v>
+        <v>135</v>
+      </c>
+      <c r="H64">
+        <v>5</v>
       </c>
       <c r="I64" t="s">
-        <v>127</v>
-      </c>
-      <c r="J64" t="s">
-        <v>127</v>
+        <v>47</v>
+      </c>
+      <c r="J64">
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -2916,10 +2928,10 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="B66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C66" t="s">
         <v>127</v>
@@ -2948,10 +2960,10 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C67" t="s">
         <v>127</v>
@@ -2980,10 +2992,10 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C68" t="s">
         <v>127</v>
@@ -3012,7 +3024,7 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -3044,10 +3056,10 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C70" t="s">
         <v>127</v>
@@ -3076,7 +3088,7 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -3108,10 +3120,10 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C72" t="s">
         <v>127</v>
@@ -3140,33 +3152,97 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>79</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73" t="s">
+        <v>127</v>
+      </c>
+      <c r="D73" t="s">
+        <v>127</v>
+      </c>
+      <c r="E73" t="s">
+        <v>127</v>
+      </c>
+      <c r="F73" t="s">
+        <v>127</v>
+      </c>
+      <c r="G73" t="s">
+        <v>127</v>
+      </c>
+      <c r="H73" t="s">
+        <v>127</v>
+      </c>
+      <c r="I73" t="s">
+        <v>127</v>
+      </c>
+      <c r="J73" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>91</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74" t="s">
+        <v>127</v>
+      </c>
+      <c r="D74" t="s">
+        <v>127</v>
+      </c>
+      <c r="E74" t="s">
+        <v>127</v>
+      </c>
+      <c r="F74" t="s">
+        <v>127</v>
+      </c>
+      <c r="G74" t="s">
+        <v>127</v>
+      </c>
+      <c r="H74" t="s">
+        <v>127</v>
+      </c>
+      <c r="I74" t="s">
+        <v>127</v>
+      </c>
+      <c r="J74" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>92</v>
       </c>
-      <c r="B73">
-        <v>0</v>
-      </c>
-      <c r="C73" t="s">
-        <v>127</v>
-      </c>
-      <c r="D73" t="s">
-        <v>127</v>
-      </c>
-      <c r="E73" t="s">
-        <v>127</v>
-      </c>
-      <c r="F73" t="s">
-        <v>127</v>
-      </c>
-      <c r="G73" t="s">
-        <v>127</v>
-      </c>
-      <c r="H73" t="s">
-        <v>127</v>
-      </c>
-      <c r="I73" t="s">
-        <v>127</v>
-      </c>
-      <c r="J73" t="s">
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75" t="s">
+        <v>127</v>
+      </c>
+      <c r="D75" t="s">
+        <v>127</v>
+      </c>
+      <c r="E75" t="s">
+        <v>127</v>
+      </c>
+      <c r="F75" t="s">
+        <v>127</v>
+      </c>
+      <c r="G75" t="s">
+        <v>127</v>
+      </c>
+      <c r="H75" t="s">
+        <v>127</v>
+      </c>
+      <c r="I75" t="s">
+        <v>127</v>
+      </c>
+      <c r="J75" t="s">
         <v>127</v>
       </c>
     </row>

</xml_diff>